<commit_message>
Added new documentation, HTML unitary test server created
</commit_message>
<xml_diff>
--- a/doc/BOM/Componentes.xlsx
+++ b/doc/BOM/Componentes.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EAD457-D6CC-467D-84C1-919F64DB46BE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFB3409-3C8F-48A8-9B1A-3B1559A07FED}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$2:$I$24</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
   <si>
     <t>Componente</t>
   </si>
@@ -68,9 +71,6 @@
   </si>
   <si>
     <t>NCP1117ST33T3G</t>
-  </si>
-  <si>
-    <t>Farnell/Aliexpress</t>
   </si>
   <si>
     <t>KM-23ID-F</t>
@@ -600,20 +600,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="5" width="40.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -621,7 +622,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -633,16 +634,16 @@
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -650,7 +651,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -680,14 +681,14 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -699,7 +700,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="1">
-        <f>H4*G4</f>
+        <f t="shared" ref="I4:I14" si="0">H4*G4</f>
         <v>1</v>
       </c>
     </row>
@@ -708,10 +709,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1">
         <v>1864742</v>
@@ -729,7 +730,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="1">
-        <f>H5*G5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -738,7 +739,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -759,7 +760,7 @@
         <v>0.121</v>
       </c>
       <c r="I6" s="1">
-        <f>H6*G6</f>
+        <f t="shared" si="0"/>
         <v>0.60499999999999998</v>
       </c>
     </row>
@@ -768,7 +769,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -777,7 +778,7 @@
         <v>1652366</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -789,16 +790,16 @@
         <v>0.36499999999999999</v>
       </c>
       <c r="I7" s="1">
-        <f>H7*G7</f>
+        <f t="shared" si="0"/>
         <v>1.825</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
@@ -807,7 +808,7 @@
         <v>2099216</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="1">
         <v>10</v>
@@ -819,16 +820,16 @@
         <v>0.13700000000000001</v>
       </c>
       <c r="I8" s="1">
-        <f>H8*G8</f>
+        <f t="shared" si="0"/>
         <v>1.37</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
@@ -837,7 +838,7 @@
         <v>2361105</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -849,16 +850,16 @@
         <v>0.97</v>
       </c>
       <c r="I9" s="1">
-        <f>H9*G9</f>
+        <f t="shared" si="0"/>
         <v>0.97</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -867,7 +868,7 @@
         <v>2610941</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
@@ -879,16 +880,16 @@
         <v>0.184</v>
       </c>
       <c r="I10" s="1">
-        <f>H10*G10</f>
+        <f t="shared" si="0"/>
         <v>0.91999999999999993</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -897,7 +898,7 @@
         <v>1972721</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" s="1">
         <v>2</v>
@@ -909,16 +910,16 @@
         <v>0.35099999999999998</v>
       </c>
       <c r="I11" s="1">
-        <f>H11*G11</f>
+        <f t="shared" si="0"/>
         <v>1.7549999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>4</v>
@@ -927,7 +928,7 @@
         <v>2782045</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
@@ -939,16 +940,16 @@
         <v>0.624</v>
       </c>
       <c r="I12" s="1">
-        <f>H12*G12</f>
+        <f t="shared" si="0"/>
         <v>0.624</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>4</v>
@@ -957,7 +958,7 @@
         <v>1022261</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="1">
         <v>2</v>
@@ -969,16 +970,16 @@
         <v>0.30199999999999999</v>
       </c>
       <c r="I13" s="1">
-        <f>H13*G13</f>
+        <f t="shared" si="0"/>
         <v>3.02</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>4</v>
@@ -987,7 +988,7 @@
         <v>2896638</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
@@ -999,16 +1000,16 @@
         <v>5.7700000000000001E-2</v>
       </c>
       <c r="I14" s="1">
-        <f>H14*G14</f>
+        <f t="shared" si="0"/>
         <v>0.57699999999999996</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
@@ -1017,7 +1018,7 @@
         <v>2896625</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" s="1">
         <v>4</v>
@@ -1029,16 +1030,16 @@
         <v>0.31900000000000001</v>
       </c>
       <c r="I15" s="1">
-        <f>G15*H15</f>
+        <f t="shared" ref="I15:I23" si="1">G15*H15</f>
         <v>1.595</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>4</v>
@@ -1047,7 +1048,7 @@
         <v>1889289</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
@@ -1059,16 +1060,16 @@
         <v>0.83399999999999996</v>
       </c>
       <c r="I16" s="1">
-        <f>G16*H16</f>
+        <f t="shared" si="1"/>
         <v>4.17</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>4</v>
@@ -1077,7 +1078,7 @@
         <v>2524677</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17" s="1">
         <v>4</v>
@@ -1089,16 +1090,16 @@
         <v>6.0400000000000002E-2</v>
       </c>
       <c r="I17" s="1">
-        <f>G17*H17</f>
+        <f t="shared" si="1"/>
         <v>0.30199999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4</v>
@@ -1107,7 +1108,7 @@
         <v>1758849</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
@@ -1119,16 +1120,16 @@
         <v>1.03E-2</v>
       </c>
       <c r="I18" s="1">
-        <f>G18*H18</f>
+        <f t="shared" si="1"/>
         <v>5.1500000000000004E-2</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
@@ -1137,7 +1138,7 @@
         <v>2861857</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19" s="1">
         <v>10</v>
@@ -1149,16 +1150,16 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I19" s="1">
-        <f>G19*H19</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>4</v>
@@ -1167,7 +1168,7 @@
         <v>2861474</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F20" s="1">
         <v>8</v>
@@ -1179,16 +1180,16 @@
         <v>7.1999999999999998E-3</v>
       </c>
       <c r="I20" s="1">
-        <f>G20*H20</f>
+        <f t="shared" si="1"/>
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>4</v>
@@ -1197,7 +1198,7 @@
         <v>2694880</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F21" s="1">
         <v>3</v>
@@ -1209,16 +1210,16 @@
         <v>5.1000000000000004E-3</v>
       </c>
       <c r="I21" s="1">
-        <f>G21*H21</f>
+        <f t="shared" si="1"/>
         <v>5.1000000000000004E-2</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>4</v>
@@ -1227,7 +1228,7 @@
         <v>2078907</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F22" s="1">
         <v>3</v>
@@ -1239,21 +1240,21 @@
         <v>1.17E-2</v>
       </c>
       <c r="I22" s="1">
-        <f>G22*H22</f>
+        <f t="shared" si="1"/>
         <v>0.11700000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F23" s="1">
         <v>1</v>
@@ -1265,7 +1266,7 @@
         <v>19.239999999999998</v>
       </c>
       <c r="I23" s="1">
-        <f>G23*H23</f>
+        <f t="shared" si="1"/>
         <v>19.239999999999998</v>
       </c>
     </row>
@@ -1277,6 +1278,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>